<commit_message>
adding edits to the postpilotedits xlsx files
</commit_message>
<xml_diff>
--- a/story_xlsx_files_postpilotiiedits/21.xlsx
+++ b/story_xlsx_files_postpilotiiedits/21.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>storyText</t>
   </si>
@@ -86,38 +86,30 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue Medium"/>
       </rPr>
-      <t>Senna got nervous about the ring, and he</t>
+      <t>While Alvira was away at the powder room, Senna took out the ring box from his jacket pocket and opened it up.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The ring contained three canary yellow diamonds that had been in his grandmother’s wedding ring. </t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="16"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve"> slipped off to the bathroom to check to make sure it looked alright.</t>
+      <t>The waiter appeared to take their order, but before Sadie got back, so that Senna could give him the ring.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The ring contained three canary yellow diamonds that had been in his grandmother’s wedding ring. </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>After Senna had gotten back to the table, the waiter appeared at their table to take their order.</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Senna ordered the oysters with garlic-parmesan sauce, and Alvira ordered the sauteed sea scallops with caramelized apples. </t>
   </si>
   <si>
     <t>“Excellent choices,” the waiter said, and he left.</t>
   </si>
   <si>
-    <t xml:space="preserve">“What a beautiful place, Senna. </t>
+    <t xml:space="preserve">“You’re too sweet, Senna. </t>
   </si>
   <si>
     <t>This is too much just to celebrate the first tomatoes I grew in the garden- really, this is absurd,” Alvira said.</t>
@@ -161,7 +153,7 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue Medium"/>
       </rPr>
-      <t>When they had finished eating, S</t>
+      <t>S</t>
     </r>
     <r>
       <rPr>
@@ -169,17 +161,14 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">enna nodded at the waiter who had been watching attentively, and he quickly strode over to place a small, elegant cake topped with the ring in front of Alvira. </t>
+      <t>enna nodded at the waiter to a small cake topped with the ring in front of Alvira, while Senna got down on one knee and asked Alvira to marry him.</t>
     </r>
   </si>
   <si>
-    <t>Her eyes widened in shock when she realized what she was looking at.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Senna got down on one knee and said,“Alvira, will you marry me? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I love you, and I will never stop loving you.” </t>
+    <t>Her eyes widened in shock when she realized what was happening.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“I love you, and I will never stop loving you,” he said. </t>
   </si>
   <si>
     <r>
@@ -188,7 +177,7 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue Medium"/>
       </rPr>
-      <t xml:space="preserve">After a few moments with everyone turned and looking at Elvira in expectation, she exclaimed, </t>
+      <t xml:space="preserve">After a few moments of silence with everyone turned and looking at Elvira in expectation, she exclaimed, </t>
     </r>
     <r>
       <rPr>
@@ -1534,7 +1523,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1918,7 +1907,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" ht="61.8" customHeight="1">
+    <row r="25" ht="79.8" customHeight="1">
       <c r="A25" t="s" s="13">
         <v>29</v>
       </c>
@@ -1933,7 +1922,7 @@
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" ht="79.8" customHeight="1">
+    <row r="26" ht="115.8" customHeight="1">
       <c r="A26" t="s" s="13">
         <v>30</v>
       </c>
@@ -1941,7 +1930,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
@@ -1963,7 +1952,7 @@
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" ht="115.8" customHeight="1">
+    <row r="28" ht="97.8" customHeight="1">
       <c r="A28" t="s" s="13">
         <v>32</v>
       </c>
@@ -1978,7 +1967,7 @@
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" ht="97.8" customHeight="1">
+    <row r="29" ht="223.8" customHeight="1">
       <c r="A29" t="s" s="13">
         <v>33</v>
       </c>
@@ -1993,7 +1982,7 @@
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" ht="223.8" customHeight="1">
+    <row r="30" ht="364.35" customHeight="1">
       <c r="A30" t="s" s="13">
         <v>34</v>
       </c>
@@ -2022,21 +2011,6 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
-    </row>
-    <row r="32" ht="364.35" customHeight="1">
-      <c r="A32" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="B32" s="9">
-        <v>4</v>
-      </c>
-      <c r="C32" s="10">
-        <v>4</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>